<commit_message>
changes made in manageclaims
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/stg/Overages/ManageInvoiceTestData.xlsx
+++ b/testdata/FCfiles/stg/Overages/ManageInvoiceTestData.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SONY\git\qualitesoft\testdata\FCfiles\stg\Overages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F85979B-6D96-4D6F-A8D8-41C77EEB58E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{8F85979B-6D96-4D6F-A8D8-41C77EEB58E4}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="3" firstSheet="1" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Validations" sheetId="2" state="hidden" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="EditSecondaryInvoice" sheetId="4" r:id="rId3"/>
-    <sheet name="EditOverageDetails" sheetId="5" r:id="rId4"/>
+    <sheet name="Validations" r:id="rId1" sheetId="2" state="hidden"/>
+    <sheet name="Sheet1" r:id="rId2" sheetId="3"/>
+    <sheet name="EditSecondaryInvoice" r:id="rId3" sheetId="4"/>
+    <sheet name="EditOverageDetails" r:id="rId4" sheetId="5"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t>Additional Handling Required</t>
   </si>
@@ -205,12 +205,46 @@
   </si>
   <si>
     <t>qashprod16sep21@mailinator.com</t>
+  </si>
+  <si>
+    <t>05-12-2022</t>
+  </si>
+  <si>
+    <t>59069890</t>
+  </si>
+  <si>
+    <t>59069894</t>
+  </si>
+  <si>
+    <t>59069895</t>
+  </si>
+  <si>
+    <t>59069896</t>
+  </si>
+  <si>
+    <t>59069900</t>
+  </si>
+  <si>
+    <t>59069901</t>
+  </si>
+  <si>
+    <t>05-13-2022</t>
+  </si>
+  <si>
+    <t>59069932</t>
+  </si>
+  <si>
+    <t>59069938</t>
+  </si>
+  <si>
+    <t>59069939</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -234,7 +268,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="60">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,8 +295,278 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -303,33 +607,249 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="36">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf applyBorder="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="3" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="5" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="7" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="9" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="11" fillId="13" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="13" fillId="15" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="17" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="19" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="19" fillId="21" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="21" fillId="23" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="23" fillId="25" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="25" fillId="27" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="27" fillId="29" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="29" fillId="31" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="31" fillId="33" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="33" fillId="35" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="35" fillId="37" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="37" fillId="39" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="39" fillId="41" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="41" fillId="43" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="43" fillId="45" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="45" fillId="47" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="47" fillId="49" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="49" fillId="51" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="51" fillId="53" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="53" fillId="55" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="55" fillId="57" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="59" borderId="57" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -414,10 +934,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -581,21 +1101,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -612,7 +1132,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -664,15 +1184,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -680,10 +1200,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="25.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="15.6" r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -713,7 +1233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="14.25" r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -739,8 +1259,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
@@ -749,8 +1269,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -758,18 +1278,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.3046875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.4375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -811,8 +1331,8 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>56</v>
+      <c r="A2" s="33" t="s">
+        <v>66</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -826,7 +1346,7 @@
       <c r="E2" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="34" t="s">
         <v>53</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -844,19 +1364,19 @@
       <c r="K2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>57</v>
+      <c r="L2" s="35" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -864,9 +1384,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -892,13 +1412,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -906,19 +1426,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="38.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1005,10 +1525,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="J2" r:id="rId2" xr:uid="{7F26AE58-39FF-430D-86E4-FA69E1224FC9}"/>
+    <hyperlink r:id="rId1" ref="L2" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink r:id="rId2" ref="J2" xr:uid="{7F26AE58-39FF-430D-86E4-FA69E1224FC9}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>